<commit_message>
#path for check and anova (done)
</commit_message>
<xml_diff>
--- a/inst/hidap/data/potato/200211/PTYL200211_CHIARA.xlsx
+++ b/inst/hidap/data/potato/200211/PTYL200211_CHIARA.xlsx
@@ -19,16 +19,16 @@
     <sheet name="Tuber_Apper" sheetId="21" r:id="rId11"/>
     <sheet name="AVDM" sheetId="22" r:id="rId12"/>
     <sheet name="ATMW" sheetId="23" r:id="rId13"/>
-    <sheet name="Plant_Vigor" sheetId="24" r:id="rId14"/>
-    <sheet name="NPH" sheetId="25" r:id="rId15"/>
-    <sheet name="NMTP" sheetId="26" r:id="rId16"/>
-    <sheet name="MTWP" sheetId="27" r:id="rId17"/>
-    <sheet name="MTYA" sheetId="28" r:id="rId18"/>
-    <sheet name="MTWPL" sheetId="29" r:id="rId19"/>
-    <sheet name="SE" sheetId="30" r:id="rId20"/>
-    <sheet name="Fieldbook" sheetId="31" r:id="rId21"/>
-    <sheet name="Summary by clone" sheetId="32" r:id="rId22"/>
-    <sheet name="Check Format" sheetId="33" r:id="rId23"/>
+    <sheet name="MTWP" sheetId="27" r:id="rId14"/>
+    <sheet name="MTYA" sheetId="28" r:id="rId15"/>
+    <sheet name="MTWPL" sheetId="29" r:id="rId16"/>
+    <sheet name="SE" sheetId="30" r:id="rId17"/>
+    <sheet name="Fieldbook" sheetId="31" r:id="rId18"/>
+    <sheet name="Summary by clone" sheetId="32" r:id="rId19"/>
+    <sheet name="Check Format" sheetId="33" r:id="rId20"/>
+    <sheet name="Plant_Vigor" sheetId="34" r:id="rId21"/>
+    <sheet name="NPH" sheetId="35" r:id="rId22"/>
+    <sheet name="NMTP" sheetId="36" r:id="rId23"/>
   </sheets>
   <definedNames>
     <definedName name="genetic_design">#REF!</definedName>
@@ -5807,7 +5807,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>870</v>
+        <v>901</v>
       </c>
     </row>
     <row r="3">
@@ -5842,7 +5842,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>873</v>
+        <v>902</v>
       </c>
     </row>
     <row r="10">
@@ -5877,7 +5877,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>541</v>
+        <v>714</v>
       </c>
     </row>
     <row r="17">
@@ -5902,437 +5902,32 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>543</v>
+        <v>865</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>875</v>
+        <v>903</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>544</v>
+        <v>866</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>876</v>
+        <v>867</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>877</v>
+        <v>904</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
         <v>878</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>882</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s">
-        <v>886</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="s">
-        <v>871</v>
       </c>
     </row>
   </sheetData>
@@ -6356,7 +5951,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>888</v>
+        <v>905</v>
       </c>
     </row>
     <row r="3">
@@ -6391,7 +5986,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>889</v>
+        <v>906</v>
       </c>
     </row>
     <row r="10">
@@ -6426,7 +6021,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>630</v>
+        <v>706</v>
       </c>
     </row>
     <row r="17">
@@ -6451,437 +6046,32 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>631</v>
+        <v>707</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>890</v>
+        <v>903</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>633</v>
+        <v>709</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>891</v>
+        <v>710</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>892</v>
+        <v>907</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
         <v>878</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="s">
-        <v>871</v>
       </c>
     </row>
   </sheetData>
@@ -6905,7 +6095,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>897</v>
+        <v>908</v>
       </c>
     </row>
     <row r="3">
@@ -6940,7 +6130,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>898</v>
+        <v>902</v>
       </c>
     </row>
     <row r="10">
@@ -6975,7 +6165,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>698</v>
+        <v>714</v>
       </c>
     </row>
     <row r="17">
@@ -7000,27 +6190,27 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>699</v>
+        <v>715</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>899</v>
+        <v>903</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>701</v>
+        <v>716</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>702</v>
+        <v>717</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>900</v>
+        <v>909</v>
       </c>
     </row>
     <row r="26">
@@ -7049,7 +6239,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
     </row>
     <row r="3">
@@ -7084,7 +6274,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>902</v>
+        <v>911</v>
       </c>
     </row>
     <row r="10">
@@ -7119,7 +6309,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>714</v>
+        <v>912</v>
       </c>
     </row>
     <row r="17">
@@ -7144,31 +6334,41 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>865</v>
+        <v>913</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>903</v>
+        <v>914</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>866</v>
+        <v>915</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>867</v>
+        <v>916</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>904</v>
+        <v>917</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
         <v>878</v>
       </c>
     </row>
@@ -7179,748 +6379,6 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>903</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>907</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>878</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>903</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>878</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="19"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="27" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="23"/>
-    </row>
-    <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="21" t="s">
-        <v>453</v>
-      </c>
-      <c r="B7" s="19"/>
-    </row>
-    <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="21" t="s">
-        <v>454</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="27" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="27" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="21" t="s">
-        <v>456</v>
-      </c>
-      <c r="B11" s="19"/>
-    </row>
-    <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="28" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="21" t="s">
-        <v>457</v>
-      </c>
-      <c r="B13" s="19"/>
-    </row>
-    <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="29" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="25" t="n">
-        <f>B14*B16*B12*B17</f>
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="24" t="n">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="24" t="n">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="30" t="n">
-        <f>(B10/B15)*10000</f>
-        <v>37037.037037037029</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="31"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="31"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="31"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="31"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="31"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" s="31"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="31"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" s="31"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" s="31"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="B28" s="31"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="26"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="B30" s="26"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="B31" s="26"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="B32" s="26"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="B33" s="26"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="B34" s="26"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="B35" s="26"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="B36" s="26"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="B37" s="26"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B38" s="26"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="B39" s="26"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="B40" s="26"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B41" s="26"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="B42" s="26"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>917</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>878</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -12580,7 +11038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -16056,6 +14514,1586 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="34.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.75" customHeight="1">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" ht="13.5" customHeight="1">
+      <c r="A3" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="19"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="27" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" ht="13.5" customHeight="1">
+      <c r="A6" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="23"/>
+    </row>
+    <row r="7" ht="13.5" customHeight="1">
+      <c r="A7" s="21" t="s">
+        <v>453</v>
+      </c>
+      <c r="B7" s="19"/>
+    </row>
+    <row r="8" ht="13.5" customHeight="1">
+      <c r="A8" s="21" t="s">
+        <v>454</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="27" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" ht="13.5" customHeight="1">
+      <c r="A11" s="21" t="s">
+        <v>456</v>
+      </c>
+      <c r="B11" s="19"/>
+    </row>
+    <row r="12" ht="13.5" customHeight="1">
+      <c r="A12" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" ht="13.5" customHeight="1">
+      <c r="A13" s="21" t="s">
+        <v>457</v>
+      </c>
+      <c r="B13" s="19"/>
+    </row>
+    <row r="14" ht="13.5" customHeight="1">
+      <c r="A14" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="29" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" ht="13.5" customHeight="1">
+      <c r="A15" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="25" t="n">
+        <f>B14*B16*B12*B17</f>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="16" ht="13.5" customHeight="1">
+      <c r="A16" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="24" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="17" ht="13.5" customHeight="1">
+      <c r="A17" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="24" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="18" ht="13.5" customHeight="1">
+      <c r="A18" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="30" t="n">
+        <f>(B10/B15)*10000</f>
+        <v>37037.037037037029</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="31"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="31"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="31"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="31"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="31"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="31"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="31"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="31"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="31"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="31"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="26"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="26"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="26"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="26"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="26"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="26"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="26"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="26"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="26"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" s="26"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="26"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="26"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="26"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>946</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>871</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>871</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
@@ -16066,175 +16104,137 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>510</v>
+        <v>869</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>919</v>
+        <v>897</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>920</v>
+        <v>869</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>919</v>
+        <v>869</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>920</v>
+        <v>871</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>919</v>
+        <v>872</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>920</v>
+        <v>871</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>921</v>
+        <v>539</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>922</v>
+        <v>898</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>923</v>
+        <v>871</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>924</v>
+        <v>869</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>925</v>
+        <v>871</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>926</v>
+        <v>874</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>927</v>
+        <v>871</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>928</v>
+        <v>540</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>929</v>
+        <v>698</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>930</v>
+        <v>871</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>931</v>
+        <v>869</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>932</v>
+        <v>542</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>933</v>
+        <v>871</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>934</v>
+        <v>699</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>935</v>
+        <v>899</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>936</v>
+        <v>701</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>937</v>
+        <v>702</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>939</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>940</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>943</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>946</v>
+        <v>878</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId5"/>
-  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
#path fixed for check and anova. #met interface
</commit_message>
<xml_diff>
--- a/inst/hidap/data/potato/200211/PTYL200211_CHIARA.xlsx
+++ b/inst/hidap/data/potato/200211/PTYL200211_CHIARA.xlsx
@@ -19,16 +19,16 @@
     <sheet name="Tuber_Apper" sheetId="21" r:id="rId11"/>
     <sheet name="AVDM" sheetId="22" r:id="rId12"/>
     <sheet name="ATMW" sheetId="23" r:id="rId13"/>
-    <sheet name="MTWP" sheetId="27" r:id="rId14"/>
-    <sheet name="MTYA" sheetId="28" r:id="rId15"/>
-    <sheet name="MTWPL" sheetId="29" r:id="rId16"/>
-    <sheet name="SE" sheetId="30" r:id="rId17"/>
-    <sheet name="Fieldbook" sheetId="31" r:id="rId18"/>
-    <sheet name="Summary by clone" sheetId="32" r:id="rId19"/>
-    <sheet name="Check Format" sheetId="33" r:id="rId20"/>
-    <sheet name="Plant_Vigor" sheetId="34" r:id="rId21"/>
-    <sheet name="NPH" sheetId="35" r:id="rId22"/>
-    <sheet name="NMTP" sheetId="36" r:id="rId23"/>
+    <sheet name="NPH" sheetId="25" r:id="rId14"/>
+    <sheet name="NMTP" sheetId="26" r:id="rId15"/>
+    <sheet name="MTWP" sheetId="27" r:id="rId16"/>
+    <sheet name="MTYA" sheetId="28" r:id="rId17"/>
+    <sheet name="MTWPL" sheetId="29" r:id="rId18"/>
+    <sheet name="Fieldbook" sheetId="31" r:id="rId19"/>
+    <sheet name="Summary by clone" sheetId="32" r:id="rId20"/>
+    <sheet name="Check Format" sheetId="33" r:id="rId21"/>
+    <sheet name="Plant_Vigor" sheetId="34" r:id="rId22"/>
+    <sheet name="SE" sheetId="35" r:id="rId23"/>
   </sheets>
   <definedNames>
     <definedName name="genetic_design">#REF!</definedName>
@@ -2920,13 +2920,13 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <color indexed="8"/>
+      <name val="Tahoma"/>
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Tahoma"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2981,12 +2981,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="43"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="22"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2995,6 +2989,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
         <bgColor indexed="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="43"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -3025,17 +3025,6 @@
       <diagonal/>
     </border>
     <border>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -3052,6 +3041,17 @@
       <left style="medium">
         <color indexed="22"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -3170,40 +3170,40 @@
   <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3211,50 +3211,50 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3263,25 +3263,25 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4117,286 +4117,286 @@
       </c>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="3"/>
     </row>
     <row r="7">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="14" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="14" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="3"/>
     </row>
     <row r="10">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="3"/>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="13" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="3"/>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="13" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="13" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="13" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="13" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="13" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="13" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="13" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="13" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="13" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="22" ht="13.5" customHeight="1">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="13" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="25" ht="13.5" customHeight="1">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="26" ht="13.5" customHeight="1">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="15" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="27" ht="13.5" customHeight="1">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="28" ht="13.5" customHeight="1">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="15" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="29" ht="13.5" customHeight="1">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="13" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="30" ht="13.5" customHeight="1">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="15" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="31" ht="13.5" customHeight="1">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="15" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="32" ht="13.5" customHeight="1">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="15" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="33" ht="13.5" customHeight="1">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="8" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="34" ht="13.5" customHeight="1">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="35" ht="13.5" customHeight="1">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="15" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="12" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="12" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="12" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="12" t="s">
         <v>358</v>
       </c>
     </row>
@@ -5807,7 +5807,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>901</v>
+        <v>888</v>
       </c>
     </row>
     <row r="3">
@@ -5842,7 +5842,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>902</v>
+        <v>889</v>
       </c>
     </row>
     <row r="10">
@@ -5877,7 +5877,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>714</v>
+        <v>630</v>
       </c>
     </row>
     <row r="17">
@@ -5902,32 +5902,437 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>865</v>
+        <v>631</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>903</v>
+        <v>890</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>866</v>
+        <v>633</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>867</v>
+        <v>891</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>904</v>
+        <v>892</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
         <v>878</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>871</v>
       </c>
     </row>
   </sheetData>
@@ -5951,7 +6356,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
     </row>
     <row r="3">
@@ -5986,7 +6391,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>906</v>
+        <v>898</v>
       </c>
     </row>
     <row r="10">
@@ -6021,7 +6426,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>706</v>
+        <v>698</v>
       </c>
     </row>
     <row r="17">
@@ -6046,27 +6451,27 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>903</v>
+        <v>899</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>709</v>
+        <v>701</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>907</v>
+        <v>900</v>
       </c>
     </row>
     <row r="26">
@@ -6095,7 +6500,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>908</v>
+        <v>901</v>
       </c>
     </row>
     <row r="3">
@@ -6190,7 +6595,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>715</v>
+        <v>865</v>
       </c>
     </row>
     <row r="22">
@@ -6200,17 +6605,17 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>716</v>
+        <v>866</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>717</v>
+        <v>867</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>909</v>
+        <v>904</v>
       </c>
     </row>
     <row r="26">
@@ -6239,7 +6644,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>910</v>
+        <v>905</v>
       </c>
     </row>
     <row r="3">
@@ -6274,7 +6679,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>911</v>
+        <v>906</v>
       </c>
     </row>
     <row r="10">
@@ -6309,7 +6714,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>912</v>
+        <v>706</v>
       </c>
     </row>
     <row r="17">
@@ -6334,41 +6739,31 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>913</v>
+        <v>707</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>914</v>
+        <v>903</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>915</v>
+        <v>709</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>916</v>
+        <v>710</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>917</v>
+        <v>907</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
         <v>878</v>
       </c>
     </row>
@@ -6379,6 +6774,150 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>878</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -11038,7 +11577,307 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="34.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.75" customHeight="1">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" ht="13.5" customHeight="1">
+      <c r="A3" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="19"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="27" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" ht="13.5" customHeight="1">
+      <c r="A6" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="23"/>
+    </row>
+    <row r="7" ht="13.5" customHeight="1">
+      <c r="A7" s="21" t="s">
+        <v>453</v>
+      </c>
+      <c r="B7" s="19"/>
+    </row>
+    <row r="8" ht="13.5" customHeight="1">
+      <c r="A8" s="21" t="s">
+        <v>454</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="27" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" ht="13.5" customHeight="1">
+      <c r="A11" s="21" t="s">
+        <v>456</v>
+      </c>
+      <c r="B11" s="19"/>
+    </row>
+    <row r="12" ht="13.5" customHeight="1">
+      <c r="A12" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" ht="13.5" customHeight="1">
+      <c r="A13" s="21" t="s">
+        <v>457</v>
+      </c>
+      <c r="B13" s="19"/>
+    </row>
+    <row r="14" ht="13.5" customHeight="1">
+      <c r="A14" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="29" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" ht="13.5" customHeight="1">
+      <c r="A15" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="25" t="n">
+        <f>B14*B16*B12*B17</f>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="16" ht="13.5" customHeight="1">
+      <c r="A16" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="24" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="17" ht="13.5" customHeight="1">
+      <c r="A17" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="24" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="18" ht="13.5" customHeight="1">
+      <c r="A18" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="30" t="n">
+        <f>(B10/B15)*10000</f>
+        <v>37037.037037037029</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="31"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="31"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="31"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="31"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="31"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="31"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="31"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="31"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="31"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="31"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="26"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="26"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="26"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="26"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="26"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="26"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="26"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="26"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="26"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" s="26"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="26"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="26"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="26"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -14514,307 +15353,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="19"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="27" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="23"/>
-    </row>
-    <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="21" t="s">
-        <v>453</v>
-      </c>
-      <c r="B7" s="19"/>
-    </row>
-    <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="21" t="s">
-        <v>454</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="27" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="27" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="21" t="s">
-        <v>456</v>
-      </c>
-      <c r="B11" s="19"/>
-    </row>
-    <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="28" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="21" t="s">
-        <v>457</v>
-      </c>
-      <c r="B13" s="19"/>
-    </row>
-    <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="29" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="25" t="n">
-        <f>B14*B16*B12*B17</f>
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="24" t="n">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="24" t="n">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="30" t="n">
-        <f>(B10/B15)*10000</f>
-        <v>37037.037037037029</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="31"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="31"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="31"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="31"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="31"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" s="31"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="31"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" s="31"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" s="31"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="B28" s="31"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="26"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="B30" s="26"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="B31" s="26"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="B32" s="26"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="B33" s="26"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="B34" s="26"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="B35" s="26"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="B36" s="26"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="B37" s="26"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B38" s="26"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="B39" s="26"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="B40" s="26"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B41" s="26"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="B42" s="26"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -14993,555 +15532,6 @@
   <tableParts count="1">
     <tablePart r:id="rId5"/>
   </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>882</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s">
-        <v>886</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="s">
-        <v>871</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -15560,7 +15550,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>888</v>
+        <v>870</v>
       </c>
     </row>
     <row r="3">
@@ -15595,7 +15585,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>889</v>
+        <v>873</v>
       </c>
     </row>
     <row r="10">
@@ -15630,7 +15620,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>630</v>
+        <v>541</v>
       </c>
     </row>
     <row r="17">
@@ -15655,27 +15645,27 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>631</v>
+        <v>543</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>890</v>
+        <v>875</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>633</v>
+        <v>544</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>891</v>
+        <v>876</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>892</v>
+        <v>877</v>
       </c>
     </row>
     <row r="26">
@@ -15725,12 +15715,12 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>893</v>
+        <v>882</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>894</v>
+        <v>883</v>
       </c>
     </row>
     <row r="37">
@@ -15765,147 +15755,147 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>895</v>
+        <v>886</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>639</v>
+        <v>550</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>640</v>
+        <v>551</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>641</v>
+        <v>552</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>642</v>
+        <v>553</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>643</v>
+        <v>554</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>644</v>
+        <v>555</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>645</v>
+        <v>556</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>646</v>
+        <v>557</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>647</v>
+        <v>558</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>648</v>
+        <v>559</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>649</v>
+        <v>560</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>650</v>
+        <v>561</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>651</v>
+        <v>562</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>652</v>
+        <v>563</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>653</v>
+        <v>564</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>654</v>
+        <v>565</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>655</v>
+        <v>566</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>656</v>
+        <v>567</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>657</v>
+        <v>568</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>658</v>
+        <v>569</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>659</v>
+        <v>570</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>660</v>
+        <v>571</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>661</v>
+        <v>572</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>662</v>
+        <v>573</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>663</v>
+        <v>574</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>664</v>
+        <v>575</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>665</v>
+        <v>576</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>666</v>
+        <v>577</v>
       </c>
     </row>
     <row r="72">
@@ -15935,147 +15925,147 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>896</v>
+        <v>887</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>668</v>
+        <v>581</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>669</v>
+        <v>582</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>670</v>
+        <v>583</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>671</v>
+        <v>584</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>672</v>
+        <v>585</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>673</v>
+        <v>586</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>674</v>
+        <v>587</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>675</v>
+        <v>588</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>676</v>
+        <v>589</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>677</v>
+        <v>590</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>678</v>
+        <v>591</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>679</v>
+        <v>592</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>680</v>
+        <v>593</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>681</v>
+        <v>594</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>682</v>
+        <v>595</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>683</v>
+        <v>596</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>684</v>
+        <v>597</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>685</v>
+        <v>598</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>686</v>
+        <v>599</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>687</v>
+        <v>600</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>688</v>
+        <v>601</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>689</v>
+        <v>602</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>690</v>
+        <v>603</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>691</v>
+        <v>604</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>692</v>
+        <v>605</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>693</v>
+        <v>606</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>694</v>
+        <v>607</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>695</v>
+        <v>608</v>
       </c>
     </row>
     <row r="106">
@@ -16109,7 +16099,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>897</v>
+        <v>910</v>
       </c>
     </row>
     <row r="3">
@@ -16144,7 +16134,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>898</v>
+        <v>911</v>
       </c>
     </row>
     <row r="10">
@@ -16179,7 +16169,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>698</v>
+        <v>912</v>
       </c>
     </row>
     <row r="17">
@@ -16204,31 +16194,41 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>699</v>
+        <v>913</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>899</v>
+        <v>914</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>701</v>
+        <v>915</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>702</v>
+        <v>916</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>900</v>
+        <v>917</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
         <v>878</v>
       </c>
     </row>
@@ -17035,7 +17035,7 @@
       <c r="E27" s="41" t="s">
         <v>445</v>
       </c>
-      <c r="F27" s="5"/>
+      <c r="F27" s="3"/>
       <c r="G27" s="42"/>
       <c r="H27" s="42" t="s">
         <v>446</v>
@@ -17831,7 +17831,7 @@
       <c r="B4" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="14" t="s">
         <v>407</v>
       </c>
       <c r="F4" s="46"/>
@@ -17840,10 +17840,10 @@
       <c r="I4" s="46"/>
     </row>
     <row r="5">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
         <v>140</v>
       </c>
       <c r="C5" t="s">
@@ -17851,10 +17851,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="13" t="s">
         <v>148</v>
       </c>
       <c r="C6" t="s">
@@ -17862,10 +17862,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="13" t="s">
         <v>160</v>
       </c>
       <c r="C7" t="s">
@@ -17873,10 +17873,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>162</v>
       </c>
       <c r="C8" t="s">
@@ -17884,10 +17884,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="13" t="s">
         <v>197</v>
       </c>
       <c r="C9" t="s">
@@ -17895,10 +17895,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="13" t="s">
         <v>225</v>
       </c>
       <c r="C10" t="s">
@@ -17906,10 +17906,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="13" t="s">
         <v>229</v>
       </c>
       <c r="C11" t="s">
@@ -17917,10 +17917,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="13" t="s">
         <v>231</v>
       </c>
       <c r="C12" t="s">
@@ -17928,10 +17928,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="13" t="s">
         <v>233</v>
       </c>
       <c r="C13" t="s">
@@ -17939,10 +17939,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="B14" s="15" t="e">
+      <c r="B14" s="13" t="e">
         <v>#N/A</v>
       </c>
       <c r="C14" t="s">
@@ -17950,10 +17950,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="B15" s="15" t="e">
+      <c r="B15" s="13" t="e">
         <v>#N/A</v>
       </c>
       <c r="C15" t="s">
@@ -18023,26 +18023,26 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="13" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="13" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
         <v>147</v>
       </c>
     </row>
@@ -18061,10 +18061,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="13" t="s">
         <v>151</v>
       </c>
     </row>
@@ -18083,10 +18083,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="13" t="s">
         <v>155</v>
       </c>
     </row>
@@ -18119,42 +18119,42 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="13" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="13" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="13" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="13" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="13" t="s">
         <v>169</v>
       </c>
     </row>
@@ -18173,42 +18173,42 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="13" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="13" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="13" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="13" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="13" t="s">
         <v>181</v>
       </c>
       <c r="C22" s="49"/>
@@ -18216,10 +18216,10 @@
       <c r="E22" s="49"/>
     </row>
     <row r="23">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="13" t="s">
         <v>183</v>
       </c>
       <c r="C23" s="49"/>
@@ -18227,10 +18227,10 @@
       <c r="E23" s="49"/>
     </row>
     <row r="24">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="13" t="s">
         <v>187</v>
       </c>
       <c r="C24" s="49"/>
@@ -18238,10 +18238,10 @@
       <c r="E24" s="49"/>
     </row>
     <row r="25">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="13" t="s">
         <v>185</v>
       </c>
       <c r="C25" s="49"/>
@@ -18329,18 +18329,18 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="13" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="13" t="s">
         <v>198</v>
       </c>
     </row>
@@ -18359,26 +18359,26 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="13" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="13" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="13" t="s">
         <v>206</v>
       </c>
     </row>
@@ -18400,50 +18400,50 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="13" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="13" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="13" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="13" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="13" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="13" t="s">
         <v>220</v>
       </c>
     </row>
@@ -18465,82 +18465,82 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="13" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="13" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="13" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="13" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="13" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="13" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="13" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="15" t="s">
+      <c r="A51" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="13" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="15" t="s">
+      <c r="A52" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="13" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="13" t="s">
         <v>242</v>
       </c>
     </row>
@@ -18562,42 +18562,42 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="15" t="s">
+      <c r="A55" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="13" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="13" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="15" t="s">
+      <c r="A57" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="B57" s="15" t="s">
+      <c r="B57" s="13" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="15" t="s">
+      <c r="A58" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B58" s="13" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="15" t="s">
+      <c r="A59" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="13" t="s">
         <v>253</v>
       </c>
     </row>

</xml_diff>